<commit_message>
Normalize all line endings using .gitattributes
</commit_message>
<xml_diff>
--- a/server/uploads/validated_output.xlsx
+++ b/server/uploads/validated_output.xlsx
@@ -502,7 +502,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -545,7 +545,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
         <v>18</v>

</xml_diff>